<commit_message>
sql files - .bacpac, .sql & .txt added
</commit_message>
<xml_diff>
--- a/database_Design/Helperland_Database.xlsx
+++ b/database_Design/Helperland_Database.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="147">
   <si>
     <t>Abhishek Vadhadiya</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t>Database for Helperland</t>
+  </si>
+  <si>
+    <t>refers to service table on which service ratting is given</t>
   </si>
 </sst>
 </file>
@@ -712,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -721,18 +724,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -742,42 +733,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -796,40 +818,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1113,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1132,46 +1136,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="52" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="50"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="28"/>
-      <c r="I4" s="10" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="39"/>
+      <c r="I4" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="28"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="39"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1180,11 +1184,11 @@
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="I5" s="12" t="s">
+      <c r="F5" s="9"/>
+      <c r="I5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="5" t="s">
@@ -1193,12 +1197,12 @@
       <c r="K5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1208,8 +1212,8 @@
         <v>23</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="13"/>
-      <c r="I6" s="14" t="s">
+      <c r="F6" s="9"/>
+      <c r="I6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="6" t="s">
@@ -1218,10 +1222,10 @@
       <c r="K6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="13"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1231,8 +1235,8 @@
         <v>24</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="13"/>
-      <c r="I7" s="14" t="s">
+      <c r="F7" s="9"/>
+      <c r="I7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J7" s="6" t="s">
@@ -1241,12 +1245,12 @@
       <c r="K7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="20"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1254,18 +1258,18 @@
         <v>25</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="13"/>
-      <c r="I8" s="14"/>
+      <c r="F8" s="9"/>
+      <c r="I8" s="10"/>
       <c r="J8" s="6" t="s">
         <v>54</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="13"/>
+      <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1277,18 +1281,18 @@
       <c r="E9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="I9" s="14"/>
+      <c r="F9" s="9"/>
+      <c r="I9" s="10"/>
       <c r="J9" s="6" t="s">
         <v>55</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="13"/>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1298,22 +1302,22 @@
         <v>26</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="13"/>
-      <c r="I10" s="16" t="s">
+      <c r="F10" s="9"/>
+      <c r="I10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1322,16 +1326,16 @@
       <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="F11" s="21"/>
+      <c r="F11" s="54"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1340,17 +1344,17 @@
       <c r="D12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="21"/>
-      <c r="I12" s="25" t="s">
+      <c r="E12" s="53"/>
+      <c r="F12" s="54"/>
+      <c r="I12" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="32"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="30"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1359,11 +1363,11 @@
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="I13" s="12" t="s">
+      <c r="F13" s="9"/>
+      <c r="I13" s="8" t="s">
         <v>1</v>
       </c>
       <c r="J13" s="5" t="s">
@@ -1372,10 +1376,10 @@
       <c r="K13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="13"/>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1384,21 +1388,23 @@
       <c r="D14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="I14" s="14"/>
+      <c r="F14" s="9"/>
+      <c r="I14" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="J14" s="7" t="s">
         <v>56</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="L14" s="13"/>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="20"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1406,18 +1412,18 @@
         <v>28</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="13"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="35" t="s">
+      <c r="F15" s="9"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="K15" s="35" t="s">
+      <c r="K15" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="24"/>
+      <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="20"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
@@ -1425,13 +1431,13 @@
         <v>27</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="13"/>
+      <c r="F16" s="9"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="20"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
@@ -1439,21 +1445,21 @@
         <v>27</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="13"/>
+      <c r="F17" s="9"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="22"/>
-      <c r="C18" s="23" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -1467,15 +1473,15 @@
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="I20" s="25" t="s">
+      <c r="I20" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="32"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="30"/>
     </row>
     <row r="21" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="15" t="s">
         <v>1</v>
       </c>
       <c r="J21" s="2" t="s">
@@ -1484,18 +1490,18 @@
       <c r="K21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L21" s="29" t="s">
+      <c r="L21" s="21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="32"/>
-      <c r="I22" s="20" t="s">
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
+      <c r="I22" s="16" t="s">
         <v>5</v>
       </c>
       <c r="J22" s="4" t="s">
@@ -1504,10 +1510,10 @@
       <c r="K22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L22" s="13"/>
+      <c r="L22" s="9"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1516,10 +1522,10 @@
       <c r="D23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="16" t="s">
         <v>19</v>
       </c>
       <c r="J23" s="4" t="s">
@@ -1528,12 +1534,12 @@
       <c r="K23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L23" s="13" t="s">
+      <c r="L23" s="9" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -1542,8 +1548,8 @@
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="I24" s="20" t="s">
+      <c r="E24" s="9"/>
+      <c r="I24" s="16" t="s">
         <v>91</v>
       </c>
       <c r="J24" s="4" t="s">
@@ -1552,12 +1558,12 @@
       <c r="K24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L24" s="13" t="s">
+      <c r="L24" s="9" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1566,10 +1572,10 @@
       <c r="D25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="16" t="s">
         <v>19</v>
       </c>
       <c r="J25" s="4" t="s">
@@ -1578,48 +1584,48 @@
       <c r="K25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L25" s="13" t="s">
+      <c r="L25" s="9" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="20"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="I26" s="20"/>
+      <c r="E26" s="9"/>
+      <c r="I26" s="16"/>
       <c r="J26" s="4" t="s">
         <v>56</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L26" s="13"/>
+      <c r="L26" s="9"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="20"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="I27" s="20"/>
+      <c r="E27" s="9"/>
+      <c r="I27" s="16"/>
       <c r="J27" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L27" s="13"/>
+      <c r="L27" s="9"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -1628,112 +1634,112 @@
       <c r="D28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="I28" s="20"/>
+      <c r="E28" s="9"/>
+      <c r="I28" s="16"/>
       <c r="J28" s="4" t="s">
         <v>64</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="L28" s="13"/>
+      <c r="L28" s="9"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="20"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="I29" s="20"/>
+      <c r="E29" s="9"/>
+      <c r="I29" s="16"/>
       <c r="J29" s="4" t="s">
         <v>65</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L29" s="13"/>
+      <c r="L29" s="9"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B30" s="20"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="I30" s="20"/>
+      <c r="E30" s="9"/>
+      <c r="I30" s="16"/>
       <c r="J30" s="4" t="s">
         <v>66</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L30" s="13"/>
+      <c r="L30" s="9"/>
     </row>
     <row r="31" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="24" t="s">
+      <c r="D31" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I31" s="20"/>
+      <c r="I31" s="16"/>
       <c r="J31" s="4" t="s">
         <v>67</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L31" s="13"/>
+      <c r="L31" s="9"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="I32" s="20"/>
+      <c r="I32" s="16"/>
       <c r="J32" s="4" t="s">
         <v>68</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L32" s="13"/>
+      <c r="L32" s="9"/>
     </row>
     <row r="33" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I33" s="20"/>
+      <c r="I33" s="16"/>
       <c r="J33" s="4" t="s">
         <v>69</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L33" s="13"/>
+      <c r="L33" s="9"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="32"/>
-      <c r="I34" s="20"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="30"/>
+      <c r="I34" s="16"/>
       <c r="J34" s="4" t="s">
         <v>124</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L34" s="13"/>
+      <c r="L34" s="9"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -1742,64 +1748,64 @@
       <c r="D35" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="29" t="s">
+      <c r="E35" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="I35" s="20"/>
+      <c r="I35" s="16"/>
       <c r="J35" s="4" t="s">
         <v>70</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L35" s="13"/>
+      <c r="L35" s="9"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="13"/>
-      <c r="I36" s="20"/>
+      <c r="E36" s="9"/>
+      <c r="I36" s="16"/>
       <c r="J36" s="4" t="s">
         <v>96</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L36" s="13"/>
+      <c r="L36" s="9"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D37" s="4"/>
-      <c r="E37" s="13"/>
-      <c r="I37" s="20"/>
+      <c r="E37" s="9"/>
+      <c r="I37" s="16"/>
       <c r="J37" s="4" t="s">
         <v>107</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L37" s="13"/>
+      <c r="L37" s="9"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B38" s="20"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="13"/>
-      <c r="I38" s="20" t="s">
+      <c r="E38" s="9"/>
+      <c r="I38" s="16" t="s">
         <v>20</v>
       </c>
       <c r="J38" s="4" t="s">
@@ -1808,18 +1814,18 @@
       <c r="K38" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L38" s="13"/>
+      <c r="L38" s="9"/>
     </row>
     <row r="39" spans="2:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="20"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="I39" s="20" t="s">
+      <c r="E39" s="9"/>
+      <c r="I39" s="16" t="s">
         <v>20</v>
       </c>
       <c r="J39" s="4" t="s">
@@ -1828,10 +1834,10 @@
       <c r="K39" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L39" s="13"/>
+      <c r="L39" s="9"/>
     </row>
     <row r="40" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -1840,8 +1846,8 @@
       <c r="D40" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="I40" s="20" t="s">
+      <c r="E40" s="9"/>
+      <c r="I40" s="16" t="s">
         <v>20</v>
       </c>
       <c r="J40" s="4" t="s">
@@ -1850,20 +1856,20 @@
       <c r="K40" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L40" s="36" t="s">
+      <c r="L40" s="40" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B41" s="20"/>
+      <c r="B41" s="16"/>
       <c r="C41" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="I41" s="20" t="s">
+      <c r="E41" s="9"/>
+      <c r="I41" s="16" t="s">
         <v>20</v>
       </c>
       <c r="J41" s="4" t="s">
@@ -1872,18 +1878,18 @@
       <c r="K41" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L41" s="36"/>
+      <c r="L41" s="40"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B42" s="20"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="I42" s="20" t="s">
+      <c r="E42" s="9"/>
+      <c r="I42" s="16" t="s">
         <v>20</v>
       </c>
       <c r="J42" s="4" t="s">
@@ -1892,50 +1898,50 @@
       <c r="K42" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L42" s="13"/>
+      <c r="L42" s="9"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B43" s="20"/>
+      <c r="B43" s="16"/>
       <c r="C43" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E43" s="13"/>
-      <c r="I43" s="20"/>
+      <c r="E43" s="9"/>
+      <c r="I43" s="16"/>
       <c r="J43" s="4" t="s">
         <v>125</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L43" s="13"/>
+      <c r="L43" s="9"/>
     </row>
     <row r="44" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="34" t="s">
+      <c r="D44" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="I44" s="22" t="s">
+      <c r="E44" s="9"/>
+      <c r="I44" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="J44" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="K44" s="23" t="s">
+      <c r="K44" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="L44" s="24"/>
+      <c r="L44" s="19"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -1944,12 +1950,12 @@
       <c r="D45" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="13"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="E45" s="9"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -1958,46 +1964,46 @@
       <c r="D46" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="13"/>
+      <c r="E46" s="9"/>
     </row>
     <row r="47" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="20"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E47" s="13"/>
+      <c r="E47" s="9"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B48" s="20"/>
+      <c r="B48" s="16"/>
       <c r="C48" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="13"/>
-      <c r="I48" s="25" t="s">
+      <c r="E48" s="9"/>
+      <c r="I48" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
-      <c r="L48" s="32"/>
+      <c r="J48" s="29"/>
+      <c r="K48" s="29"/>
+      <c r="L48" s="30"/>
     </row>
     <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="22"/>
-      <c r="C49" s="23" t="s">
+      <c r="B49" s="17"/>
+      <c r="C49" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E49" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="I49" s="19" t="s">
+      <c r="I49" s="15" t="s">
         <v>1</v>
       </c>
       <c r="J49" s="2" t="s">
@@ -2006,12 +2012,12 @@
       <c r="K49" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L49" s="29" t="s">
+      <c r="L49" s="21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I50" s="20" t="s">
+      <c r="I50" s="16" t="s">
         <v>5</v>
       </c>
       <c r="J50" s="4" t="s">
@@ -2020,27 +2026,27 @@
       <c r="K50" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L50" s="13"/>
+      <c r="L50" s="9"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="32"/>
-      <c r="I51" s="20" t="s">
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="30"/>
+      <c r="I51" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="J51" s="34" t="s">
+      <c r="J51" s="23" t="s">
         <v>120</v>
       </c>
       <c r="K51" s="4"/>
-      <c r="L51" s="13"/>
+      <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A52" s="20"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
@@ -2050,20 +2056,20 @@
       <c r="D52" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="29" t="s">
+      <c r="E52" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="I52" s="20" t="s">
+      <c r="I52" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J52" s="34" t="s">
+      <c r="J52" s="23" t="s">
         <v>74</v>
       </c>
       <c r="K52" s="4"/>
-      <c r="L52" s="13"/>
+      <c r="L52" s="9"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="51" t="s">
         <v>95</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -2075,10 +2081,10 @@
       <c r="D53" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="I53" s="20" t="s">
+      <c r="I53" s="16" t="s">
         <v>19</v>
       </c>
       <c r="J53" s="4" t="s">
@@ -2087,58 +2093,58 @@
       <c r="K53" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L53" s="13" t="s">
+      <c r="L53" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="31"/>
-      <c r="B54" s="23" t="s">
+      <c r="A54" s="52"/>
+      <c r="B54" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="23" t="s">
+      <c r="C54" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D54" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E54" s="24" t="s">
+      <c r="D54" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="I54" s="20"/>
+      <c r="I54" s="16"/>
       <c r="J54" s="4" t="s">
         <v>75</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L54" s="13"/>
+      <c r="L54" s="9"/>
     </row>
     <row r="55" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I55" s="22" t="s">
+      <c r="I55" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J55" s="23" t="s">
+      <c r="J55" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="K55" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="L55" s="24" t="s">
+      <c r="K55" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L55" s="19" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="32"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="30"/>
     </row>
     <row r="57" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="20"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="1" t="s">
         <v>1</v>
       </c>
@@ -2148,12 +2154,12 @@
       <c r="D57" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E57" s="29" t="s">
+      <c r="E57" s="21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="51" t="s">
         <v>95</v>
       </c>
       <c r="B58" s="4" t="s">
@@ -2165,31 +2171,31 @@
       <c r="D58" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="I58" s="25" t="s">
+      <c r="I58" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="J58" s="26"/>
-      <c r="K58" s="26"/>
-      <c r="L58" s="32"/>
+      <c r="J58" s="29"/>
+      <c r="K58" s="29"/>
+      <c r="L58" s="30"/>
     </row>
     <row r="59" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="31"/>
-      <c r="B59" s="23" t="s">
+      <c r="A59" s="52"/>
+      <c r="B59" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="23" t="s">
+      <c r="C59" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D59" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E59" s="24" t="s">
+      <c r="D59" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E59" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I59" s="19" t="s">
+      <c r="I59" s="15" t="s">
         <v>1</v>
       </c>
       <c r="J59" s="2" t="s">
@@ -2198,12 +2204,12 @@
       <c r="K59" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L59" s="29" t="s">
+      <c r="L59" s="21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="I60" s="20" t="s">
+      <c r="I60" s="16" t="s">
         <v>5</v>
       </c>
       <c r="J60" s="4" t="s">
@@ -2212,10 +2218,10 @@
       <c r="K60" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L60" s="13"/>
+      <c r="L60" s="9"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="I61" s="20" t="s">
+      <c r="I61" s="16" t="s">
         <v>19</v>
       </c>
       <c r="J61" s="4" t="s">
@@ -2224,12 +2230,12 @@
       <c r="K61" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L61" s="13" t="s">
+      <c r="L61" s="9" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="I62" s="20" t="s">
+      <c r="I62" s="16" t="s">
         <v>19</v>
       </c>
       <c r="J62" s="4" t="s">
@@ -2238,42 +2244,42 @@
       <c r="K62" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L62" s="13" t="s">
+      <c r="L62" s="9" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I63" s="20"/>
+      <c r="I63" s="16"/>
       <c r="J63" s="4" t="s">
         <v>84</v>
       </c>
       <c r="K63" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L63" s="13" t="s">
+      <c r="L63" s="9" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B64" s="25" t="s">
+      <c r="B64" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="26"/>
-      <c r="D64" s="26"/>
-      <c r="E64" s="32"/>
-      <c r="I64" s="20"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="30"/>
+      <c r="I64" s="16"/>
       <c r="J64" s="4" t="s">
         <v>85</v>
       </c>
       <c r="K64" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L64" s="13" t="s">
+      <c r="L64" s="9" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B65" s="19" t="s">
+      <c r="B65" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -2282,22 +2288,22 @@
       <c r="D65" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E65" s="46" t="s">
+      <c r="E65" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="I65" s="20"/>
+      <c r="I65" s="16"/>
       <c r="J65" s="4" t="s">
         <v>86</v>
       </c>
       <c r="K65" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L65" s="13" t="s">
+      <c r="L65" s="9" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="4" t="s">
@@ -2306,61 +2312,75 @@
       <c r="D66" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E66" s="46"/>
-      <c r="I66" s="20"/>
-      <c r="J66" s="4" t="s">
+      <c r="E66" s="26"/>
+      <c r="I66" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J66" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="K66" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L66" s="55" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B67" s="17"/>
+      <c r="C67" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E67" s="27"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="K66" s="4" t="s">
+      <c r="K67" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="L66" s="13"/>
-    </row>
-    <row r="67" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B67" s="22"/>
-      <c r="C67" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D67" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E67" s="47"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="23" t="s">
+      <c r="L67" s="9"/>
+    </row>
+    <row r="68" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I68" s="17"/>
+      <c r="J68" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="K67" s="23" t="s">
+      <c r="K68" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="L67" s="24"/>
+      <c r="L68" s="19"/>
     </row>
     <row r="69" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="70" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I70" s="25" t="s">
+      <c r="I70" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="J70" s="26"/>
-      <c r="K70" s="32"/>
+      <c r="J70" s="29"/>
+      <c r="K70" s="30"/>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B71" s="25" t="s">
+      <c r="B71" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C71" s="26"/>
-      <c r="D71" s="26"/>
-      <c r="E71" s="32"/>
-      <c r="I71" s="19" t="s">
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="30"/>
+      <c r="I71" s="15" t="s">
         <v>1</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K71" s="33" t="s">
+      <c r="K71" s="22" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B72" s="19" t="s">
+      <c r="B72" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C72" s="2" t="s">
@@ -2369,21 +2389,21 @@
       <c r="D72" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E72" s="29" t="s">
+      <c r="E72" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="I72" s="20" t="s">
+      <c r="I72" s="16" t="s">
         <v>5</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="K72" s="13" t="s">
+      <c r="K72" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="4" t="s">
@@ -2392,192 +2412,192 @@
       <c r="D73" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E73" s="13"/>
-      <c r="I73" s="20"/>
+      <c r="E73" s="9"/>
+      <c r="I73" s="16"/>
       <c r="J73" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K73" s="13" t="s">
+      <c r="K73" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B74" s="20"/>
+      <c r="B74" s="16"/>
       <c r="C74" s="4" t="s">
         <v>103</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E74" s="13" t="s">
+      <c r="E74" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="I74" s="20"/>
+      <c r="I74" s="16"/>
       <c r="J74" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="K74" s="13" t="s">
+      <c r="K74" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B75" s="20"/>
+      <c r="B75" s="16"/>
       <c r="C75" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E75" s="13"/>
-      <c r="I75" s="20"/>
+      <c r="E75" s="9"/>
+      <c r="I75" s="16"/>
       <c r="J75" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K75" s="13" t="s">
+      <c r="K75" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="76" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B76" s="22"/>
-      <c r="C76" s="48" t="s">
+      <c r="B76" s="17"/>
+      <c r="C76" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D76" s="48" t="s">
+      <c r="D76" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E76" s="24" t="s">
+      <c r="E76" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="I76" s="20"/>
+      <c r="I76" s="16"/>
       <c r="J76" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="K76" s="13" t="s">
+      <c r="K76" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="I77" s="20"/>
+      <c r="I77" s="16"/>
       <c r="J77" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K77" s="13" t="s">
+      <c r="K77" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="78" spans="2:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I78" s="22"/>
-      <c r="J78" s="23" t="s">
+      <c r="I78" s="17"/>
+      <c r="J78" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="K78" s="24" t="s">
+      <c r="K78" s="19" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B79" s="43" t="s">
+      <c r="B79" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C79" s="44"/>
-      <c r="D79" s="44"/>
-      <c r="E79" s="45"/>
+      <c r="C79" s="42"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="43"/>
     </row>
     <row r="80" spans="2:12" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B80" s="37" t="s">
+      <c r="B80" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="C80" s="38"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="39"/>
+      <c r="C80" s="45"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="46"/>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B81" s="37"/>
-      <c r="C81" s="38"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="39"/>
-      <c r="I81" s="49" t="s">
+      <c r="B81" s="44"/>
+      <c r="C81" s="45"/>
+      <c r="D81" s="45"/>
+      <c r="E81" s="46"/>
+      <c r="I81" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="J81" s="50"/>
-      <c r="K81" s="51"/>
+      <c r="J81" s="32"/>
+      <c r="K81" s="33"/>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B82" s="37"/>
-      <c r="C82" s="38"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="39"/>
-      <c r="I82" s="20" t="s">
+      <c r="B82" s="44"/>
+      <c r="C82" s="45"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="46"/>
+      <c r="I82" s="16" t="s">
         <v>18</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="K82" s="13" t="s">
+      <c r="K82" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="83" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B83" s="40"/>
-      <c r="C83" s="41"/>
-      <c r="D83" s="41"/>
-      <c r="E83" s="42"/>
-      <c r="I83" s="20" t="s">
+      <c r="B83" s="47"/>
+      <c r="C83" s="48"/>
+      <c r="D83" s="48"/>
+      <c r="E83" s="49"/>
+      <c r="I83" s="16" t="s">
         <v>20</v>
       </c>
       <c r="J83" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="K83" s="13" t="s">
+      <c r="K83" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="I84" s="20"/>
+      <c r="I84" s="16"/>
       <c r="J84" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="K84" s="13" t="s">
+      <c r="K84" s="9" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="85" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I85" s="22" t="s">
+      <c r="I85" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J85" s="23" t="s">
+      <c r="J85" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="K85" s="24" t="s">
+      <c r="K85" s="19" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A53:A54"/>
     <mergeCell ref="E65:E67"/>
     <mergeCell ref="B64:E64"/>
     <mergeCell ref="I81:K81"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="B4:F4"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A56:E56"/>
     <mergeCell ref="B71:E71"/>
     <mergeCell ref="B79:E79"/>
     <mergeCell ref="B80:E83"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A53:A54"/>
     <mergeCell ref="I70:K70"/>
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="E11:F12"/>
     <mergeCell ref="I58:L58"/>
     <mergeCell ref="I20:L20"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="I48:L48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>